<commit_message>
Completed first public version
</commit_message>
<xml_diff>
--- a/output/ROS_Variable_Dictionary.xlsx
+++ b/output/ROS_Variable_Dictionary.xlsx
@@ -9891,12 +9891,12 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>m2a1</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>m1. nom des personnes du ménage</t>
+          <t>m2a1. statut de résidence</t>
         </is>
       </c>
       <c r="D434" t="inlineStr">
@@ -9913,12 +9913,12 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>m2a1</t>
+          <t>m3</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>m2a1. statut de résidence</t>
+          <t>m3. si absent, raison de l'absence</t>
         </is>
       </c>
       <c r="D435" t="inlineStr">
@@ -9935,12 +9935,12 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>m3</t>
+          <t>m4</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>m3. si absent, raison de l'absence</t>
+          <t>m4. quel est le sexe de ' nom ' ?</t>
         </is>
       </c>
       <c r="D436" t="inlineStr">
@@ -9957,12 +9957,12 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>m4</t>
+          <t>m5</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>m4. quel est le sexe de ' nom ' ?</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="D437" t="inlineStr">
@@ -9979,12 +9979,12 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>m5</t>
+          <t>m6</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>m5. age de ' nom ' ?</t>
+          <t>m6. quel est le lien de parenté de ' nom ' avec le chef de ménage ?</t>
         </is>
       </c>
       <c r="D438" t="inlineStr">
@@ -10001,12 +10001,12 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>m6</t>
+          <t>m7</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>m6. quel est le lien de parenté de ' nom ' avec le chef de ménage ?</t>
+          <t>m7. quelle est la situation de famille de ' nom ' ?</t>
         </is>
       </c>
       <c r="D439" t="inlineStr">
@@ -10023,12 +10023,12 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>m7</t>
+          <t>m8b</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>m7. quelle est la situation de famille de ' nom ' ?</t>
+          <t>m8b. lieu de naissance</t>
         </is>
       </c>
       <c r="D440" t="inlineStr">
@@ -10045,12 +10045,12 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>m8b</t>
+          <t>m9a</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>m8b. lieu de naissance</t>
+          <t>m9a. nationalité</t>
         </is>
       </c>
       <c r="D441" t="inlineStr">
@@ -10067,12 +10067,12 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>m9a</t>
+          <t>m9b</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>m9a. nationalité</t>
+          <t>m9b. religion</t>
         </is>
       </c>
       <c r="D442" t="inlineStr">
@@ -10089,12 +10089,12 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>m9b</t>
+          <t>mg4b</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>m9b. religion</t>
+          <t>mg4b. ethnie</t>
         </is>
       </c>
       <c r="D443" t="inlineStr">
@@ -10111,12 +10111,12 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>mg4b</t>
+          <t>mi1</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>mg4b. ethnie</t>
+          <t>mi1. déplacez-vous hors de la région durant plusieurs semaines pour le travail ?</t>
         </is>
       </c>
       <c r="D444" t="inlineStr">
@@ -10133,12 +10133,12 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>mi1</t>
+          <t>mi2</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>mi1. déplacez-vous hors de la région durant plusieurs semaines pour le travail ?</t>
+          <t>mi2. lieu de déplacement</t>
         </is>
       </c>
       <c r="D445" t="inlineStr">
@@ -10155,12 +10155,12 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>mi2</t>
+          <t>mi3</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>mi2. lieu de déplacement</t>
+          <t>mi3. durée (en semaines)</t>
         </is>
       </c>
       <c r="D446" t="inlineStr">
@@ -10177,12 +10177,12 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>mi3</t>
+          <t>mi4</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>mi3. durée (en semaines)</t>
+          <t>mi4. pour quel type d'activité</t>
         </is>
       </c>
       <c r="D447" t="inlineStr">
@@ -10199,12 +10199,12 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>mi4</t>
+          <t>obsr</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>mi4. pour quel type d'activité</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="D448" t="inlineStr">
@@ -10221,7 +10221,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>obsr</t>
+          <t>pseudonym</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
@@ -20803,17 +20803,17 @@
       </c>
       <c r="B930" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>m11</t>
         </is>
       </c>
       <c r="C930" t="inlineStr">
         <is>
-          <t>m1. nom des personnes du ménage</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="D930" t="inlineStr">
         <is>
-          <t>1996,1997,1998,1999,2000,2001,2002,2003,2004,2005,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
+          <t>1996,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
         </is>
       </c>
     </row>
@@ -20825,17 +20825,17 @@
       </c>
       <c r="B931" t="inlineStr">
         <is>
-          <t>m11</t>
+          <t>m2a1</t>
         </is>
       </c>
       <c r="C931" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>m2a1. statut de résidence</t>
         </is>
       </c>
       <c r="D931" t="inlineStr">
         <is>
-          <t>1996,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
+          <t>1996,1997</t>
         </is>
       </c>
     </row>
@@ -20847,17 +20847,17 @@
       </c>
       <c r="B932" t="inlineStr">
         <is>
-          <t>m2a1</t>
+          <t>m2d</t>
         </is>
       </c>
       <c r="C932" t="inlineStr">
         <is>
-          <t>m2a1. statut de résidence</t>
+          <t>m2d. nouveau membre du ménage venu par</t>
         </is>
       </c>
       <c r="D932" t="inlineStr">
         <is>
-          <t>1996,1997</t>
+          <t>1996,1997,2005,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
         </is>
       </c>
     </row>
@@ -20869,17 +20869,17 @@
       </c>
       <c r="B933" t="inlineStr">
         <is>
-          <t>m2d</t>
+          <t>m3</t>
         </is>
       </c>
       <c r="C933" t="inlineStr">
         <is>
-          <t>m2d. nouveau membre du ménage venu par</t>
+          <t>m3. si absent, raison de l'absence</t>
         </is>
       </c>
       <c r="D933" t="inlineStr">
         <is>
-          <t>1996,1997,2005,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
+          <t>1996,1997</t>
         </is>
       </c>
     </row>
@@ -20891,17 +20891,17 @@
       </c>
       <c r="B934" t="inlineStr">
         <is>
-          <t>m3</t>
+          <t>m4</t>
         </is>
       </c>
       <c r="C934" t="inlineStr">
         <is>
-          <t>m3. si absent, raison de l'absence</t>
+          <t>m4. quel est le sexe de ' nom ' ?</t>
         </is>
       </c>
       <c r="D934" t="inlineStr">
         <is>
-          <t>1996,1997</t>
+          <t>1996,1997,1998,1999,2000,2001,2002,2003,2004,2005,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
         </is>
       </c>
     </row>
@@ -20913,12 +20913,12 @@
       </c>
       <c r="B935" t="inlineStr">
         <is>
-          <t>m4</t>
+          <t>m5</t>
         </is>
       </c>
       <c r="C935" t="inlineStr">
         <is>
-          <t>m4. quel est le sexe de ' nom ' ?</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="D935" t="inlineStr">
@@ -20935,12 +20935,12 @@
       </c>
       <c r="B936" t="inlineStr">
         <is>
-          <t>m5</t>
+          <t>m6</t>
         </is>
       </c>
       <c r="C936" t="inlineStr">
         <is>
-          <t>m5. age de ' nom ' ?</t>
+          <t>m6. quel est le lien de parenté de ' nom ' avec le chef de ménage ?</t>
         </is>
       </c>
       <c r="D936" t="inlineStr">
@@ -20957,12 +20957,12 @@
       </c>
       <c r="B937" t="inlineStr">
         <is>
-          <t>m6</t>
+          <t>m7</t>
         </is>
       </c>
       <c r="C937" t="inlineStr">
         <is>
-          <t>m6. quel est le lien de parenté de ' nom ' avec le chef de ménage ?</t>
+          <t>m7. quelle est la situation de famille de ' nom ' ?</t>
         </is>
       </c>
       <c r="D937" t="inlineStr">
@@ -20979,17 +20979,17 @@
       </c>
       <c r="B938" t="inlineStr">
         <is>
-          <t>m7</t>
+          <t>m9b</t>
         </is>
       </c>
       <c r="C938" t="inlineStr">
         <is>
-          <t>m7. quelle est la situation de famille de ' nom ' ?</t>
+          <t>m9b. religion</t>
         </is>
       </c>
       <c r="D938" t="inlineStr">
         <is>
-          <t>1996,1997,1998,1999,2000,2001,2002,2003,2004,2005,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
+          <t>1996</t>
         </is>
       </c>
     </row>
@@ -21001,17 +21001,17 @@
       </c>
       <c r="B939" t="inlineStr">
         <is>
-          <t>m9b</t>
+          <t>mg4b</t>
         </is>
       </c>
       <c r="C939" t="inlineStr">
         <is>
-          <t>m9b. religion</t>
+          <t>mg4b. ethnie</t>
         </is>
       </c>
       <c r="D939" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>1996,1997,1998,1999,2000,2001,2010,2011,2012</t>
         </is>
       </c>
     </row>
@@ -21023,17 +21023,17 @@
       </c>
       <c r="B940" t="inlineStr">
         <is>
-          <t>mg4b</t>
+          <t>mi2</t>
         </is>
       </c>
       <c r="C940" t="inlineStr">
         <is>
-          <t>mg4b. ethnie</t>
+          <t>mi2. lieu de migration saisonnière</t>
         </is>
       </c>
       <c r="D940" t="inlineStr">
         <is>
-          <t>1996,1997,1998,1999,2000,2001,2010,2011,2012</t>
+          <t>1996</t>
         </is>
       </c>
     </row>
@@ -21045,12 +21045,12 @@
       </c>
       <c r="B941" t="inlineStr">
         <is>
-          <t>mi2</t>
+          <t>mi2a</t>
         </is>
       </c>
       <c r="C941" t="inlineStr">
         <is>
-          <t>mi2. lieu de migration saisonnière</t>
+          <t>mi2a. départ (mois)</t>
         </is>
       </c>
       <c r="D941" t="inlineStr">
@@ -21067,12 +21067,12 @@
       </c>
       <c r="B942" t="inlineStr">
         <is>
-          <t>mi2a</t>
+          <t>mi3</t>
         </is>
       </c>
       <c r="C942" t="inlineStr">
         <is>
-          <t>mi2a. départ (mois)</t>
+          <t>mi3. durée (en semaines)</t>
         </is>
       </c>
       <c r="D942" t="inlineStr">
@@ -21089,12 +21089,12 @@
       </c>
       <c r="B943" t="inlineStr">
         <is>
-          <t>mi3</t>
+          <t>mi4a</t>
         </is>
       </c>
       <c r="C943" t="inlineStr">
         <is>
-          <t>mi3. durée (en semaines)</t>
+          <t>mi4a. motif</t>
         </is>
       </c>
       <c r="D943" t="inlineStr">
@@ -21111,12 +21111,12 @@
       </c>
       <c r="B944" t="inlineStr">
         <is>
-          <t>mi4a</t>
+          <t>mi5</t>
         </is>
       </c>
       <c r="C944" t="inlineStr">
         <is>
-          <t>mi4a. motif</t>
+          <t>mi5. moyen de déplacement</t>
         </is>
       </c>
       <c r="D944" t="inlineStr">
@@ -21133,12 +21133,12 @@
       </c>
       <c r="B945" t="inlineStr">
         <is>
-          <t>mi5</t>
+          <t>obsr96</t>
         </is>
       </c>
       <c r="C945" t="inlineStr">
         <is>
-          <t>mi5. moyen de déplacement</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="D945" t="inlineStr">
@@ -21155,7 +21155,7 @@
       </c>
       <c r="B946" t="inlineStr">
         <is>
-          <t>obsr96</t>
+          <t>pseudonym</t>
         </is>
       </c>
       <c r="C946" t="inlineStr">
@@ -21165,7 +21165,7 @@
       </c>
       <c r="D946" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>1996,1997,1998,1999,2000,2001,2002,2003,2004,2005,2006,2007,2008,2009,2010,2011,2012,2013,2014,2015</t>
         </is>
       </c>
     </row>

</xml_diff>